<commit_message>
Improved Data Driven Approach
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/BestBuy/Data/Test Data.xlsx
+++ b/src/main/java/com/qa/BestBuy/Data/Test Data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101139\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDD9928-245B-4ECB-B9A8-1884D3045FD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A2509A-040A-4ADF-865F-D25779D09B81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260C3086-3511-4230-BA70-4E79DBD493AE}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>